<commit_message>
Mise à jour du modèle logique avec des exemples (#94)
* update ml

* update poso

* fix typo

* update typo

* fix another typo

* update seq

* ajout lien xt ehr

* update poso

* test example b3c8ce7c097c16400a58ef9cff13b03d1accb2de
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-ligne-prescription.xlsx
+++ b/main/ig/StructureDefinition-fr-ligne-prescription.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Ligne de precription</t>
+    <t>Ligne de prescription</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-22T19:10:19+00:00</t>
+    <t>2025-07-31T09:35:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Structuration d'une ligne de prescription [à compléter].</t>
+    <t>Structuration d'une ligne de prescription [WIP - à compléter].</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>